<commit_message>
Merged to Master branch (but with errors. Bugs created)
</commit_message>
<xml_diff>
--- a/examples/simpleAutomationpractice.xlsx
+++ b/examples/simpleAutomationpractice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71584B8-C72B-BF46-BD90-2FAC5C342983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A041F03-B087-1149-A600-E02A9387F7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Activity</t>
   </si>
@@ -77,35 +77,80 @@
     <t>SETTEXT</t>
   </si>
   <si>
-    <t>franzi@mailinator.com</t>
-  </si>
-  <si>
     <t>//*[@id='id_order']</t>
   </si>
   <si>
-    <t>fritzi</t>
-  </si>
-  <si>
     <t>//*[@id='message']</t>
   </si>
   <si>
-    <t>Testmessage message message</t>
-  </si>
-  <si>
     <t>//button[@id='submitMessage']/span</t>
   </si>
   <si>
     <t>//div[@id='center_column']/ul/li/a/span</t>
   </si>
   <si>
-    <t>Dummy</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>$(Email)</t>
+  </si>
+  <si>
+    <t>$(Name)</t>
+  </si>
+  <si>
+    <t>$(Message)</t>
+  </si>
+  <si>
+    <t>Good@baangt.org</t>
+  </si>
+  <si>
+    <t>Tests@baangt.org</t>
+  </si>
+  <si>
+    <t>Let@baangt.org</t>
+  </si>
+  <si>
+    <t>you@baangt.org</t>
+  </si>
+  <si>
+    <t>sleep@baangt.org</t>
+  </si>
+  <si>
+    <t>well@baangt.org</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Let</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>Good Tests let you sleep well</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +165,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,15 +204,41 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -164,6 +249,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204AEBD8-FB75-1940-BD5B-BEB77C95C906}" name="Tabelle1" displayName="Tabelle1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I13" xr:uid="{785075D4-54D6-3C41-81C4-1E0DDD8F532E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2CAEB1B0-3AE0-5C4E-96E3-EA9525E8AF80}" name="Activity"/>
+    <tableColumn id="2" xr3:uid="{DA1FA16C-0606-F94E-A8F4-A317FCFB6375}" name="LocatorType"/>
+    <tableColumn id="3" xr3:uid="{278C21A2-2DAB-8647-B34D-E42A9EC98A1B}" name="Locator"/>
+    <tableColumn id="4" xr3:uid="{F0534D96-4CE7-4347-870A-563C9B5DF196}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{39E9D7A6-DDEB-ED4D-9C68-DAEED701776D}" name="Comparison"/>
+    <tableColumn id="6" xr3:uid="{387CCBF5-B0E6-1147-B44D-79D3E19F8FAC}" name="Value2"/>
+    <tableColumn id="7" xr3:uid="{FA69292C-F50A-8844-B3AB-1FBA0AE89958}" name="Timeout"/>
+    <tableColumn id="8" xr3:uid="{1A15E922-C36E-844E-88D8-B59A9862000A}" name="Optional"/>
+    <tableColumn id="9" xr3:uid="{76B72869-30E0-F144-B25E-8C950FD007F3}" name="Release"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,36 +592,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -554,6 +665,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -588,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -599,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -610,10 +724,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -624,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -635,10 +749,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -649,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -660,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -668,75 +782,112 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE42C928-68C5-8348-BC97-B630FA619B5E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F7C124DA-23C1-EE4F-8958-30428CC233A4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{DE82AA97-E5C6-134A-96C0-5DB4BD705B33}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{1DFD3490-645E-434A-A42A-E5911F9D4B82}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{C4CE511D-B226-D344-A384-7E6AF3BE221F}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{686012E0-067E-E74E-8ECA-D187B02BA5C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nicer format of XLSX
</commit_message>
<xml_diff>
--- a/examples/simpleAutomationpractice.xlsx
+++ b/examples/simpleAutomationpractice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71584B8-C72B-BF46-BD90-2FAC5C342983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A041F03-B087-1149-A600-E02A9387F7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Activity</t>
   </si>
@@ -77,35 +77,80 @@
     <t>SETTEXT</t>
   </si>
   <si>
-    <t>franzi@mailinator.com</t>
-  </si>
-  <si>
     <t>//*[@id='id_order']</t>
   </si>
   <si>
-    <t>fritzi</t>
-  </si>
-  <si>
     <t>//*[@id='message']</t>
   </si>
   <si>
-    <t>Testmessage message message</t>
-  </si>
-  <si>
     <t>//button[@id='submitMessage']/span</t>
   </si>
   <si>
     <t>//div[@id='center_column']/ul/li/a/span</t>
   </si>
   <si>
-    <t>Dummy</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>$(Email)</t>
+  </si>
+  <si>
+    <t>$(Name)</t>
+  </si>
+  <si>
+    <t>$(Message)</t>
+  </si>
+  <si>
+    <t>Good@baangt.org</t>
+  </si>
+  <si>
+    <t>Tests@baangt.org</t>
+  </si>
+  <si>
+    <t>Let@baangt.org</t>
+  </si>
+  <si>
+    <t>you@baangt.org</t>
+  </si>
+  <si>
+    <t>sleep@baangt.org</t>
+  </si>
+  <si>
+    <t>well@baangt.org</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Let</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>Good Tests let you sleep well</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +165,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,15 +204,41 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -164,6 +249,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204AEBD8-FB75-1940-BD5B-BEB77C95C906}" name="Tabelle1" displayName="Tabelle1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I13" xr:uid="{785075D4-54D6-3C41-81C4-1E0DDD8F532E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2CAEB1B0-3AE0-5C4E-96E3-EA9525E8AF80}" name="Activity"/>
+    <tableColumn id="2" xr3:uid="{DA1FA16C-0606-F94E-A8F4-A317FCFB6375}" name="LocatorType"/>
+    <tableColumn id="3" xr3:uid="{278C21A2-2DAB-8647-B34D-E42A9EC98A1B}" name="Locator"/>
+    <tableColumn id="4" xr3:uid="{F0534D96-4CE7-4347-870A-563C9B5DF196}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{39E9D7A6-DDEB-ED4D-9C68-DAEED701776D}" name="Comparison"/>
+    <tableColumn id="6" xr3:uid="{387CCBF5-B0E6-1147-B44D-79D3E19F8FAC}" name="Value2"/>
+    <tableColumn id="7" xr3:uid="{FA69292C-F50A-8844-B3AB-1FBA0AE89958}" name="Timeout"/>
+    <tableColumn id="8" xr3:uid="{1A15E922-C36E-844E-88D8-B59A9862000A}" name="Optional"/>
+    <tableColumn id="9" xr3:uid="{76B72869-30E0-F144-B25E-8C950FD007F3}" name="Release"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,36 +592,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -554,6 +665,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -588,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -599,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -610,10 +724,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -624,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -635,10 +749,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -649,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -660,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -668,75 +782,112 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE42C928-68C5-8348-BC97-B630FA619B5E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F7C124DA-23C1-EE4F-8958-30428CC233A4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{DE82AA97-E5C6-134A-96C0-5DB4BD705B33}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{1DFD3490-645E-434A-A42A-E5911F9D4B82}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{C4CE511D-B226-D344-A384-7E6AF3BE221F}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{686012E0-067E-E74E-8ECA-D187B02BA5C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>